<commit_message>
Time History aktualisiert, Diagramm verschönert !! Keine Veränderungen am Programm vorgenommen !!
</commit_message>
<xml_diff>
--- a/Time_Histroy.xlsx
+++ b/Time_Histroy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://htlr-my.sharepoint.com/personal/stefan_lins_student_htl-rankweil_at/Documents/SJ_2022_23/Labor/5_Trenkwaldr/Conway/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\Desktop\Neuer Ordner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_AD4DB114E441178AC67DF47DE691FD58683EDF10" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57A34375-EC86-4C67-ACC0-E6AE78C61D31}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D569E0CB-4E5B-4C5A-8486-E00D4E03044B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Anfangsprogramm</t>
   </si>
@@ -33,20 +33,26 @@
     <t>Anfangsprogramm mit Kopileroptimierung</t>
   </si>
   <si>
-    <t>initSpielfeld gelöscht</t>
-  </si>
-  <si>
     <t>pruefeRegeln überarbeitet</t>
   </si>
   <si>
-    <t>X,Y Anzeige &amp; Lebende Anzeige entfert</t>
+    <t>initSpielefeld gelöscht</t>
+  </si>
+  <si>
+    <t>X,Y Anzeige links oben entfernt</t>
+  </si>
+  <si>
+    <t>Zähllebende und FindNachbar zusammengefasst, Funktionsaufrufe entfernen</t>
+  </si>
+  <si>
+    <t>Datentypen optimert, Funktionsaufruf pruefeRegeln entfernt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,10 +61,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF656D76"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,19 +101,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -141,7 +171,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-AT"/>
-              <a:t>Südr</a:t>
+              <a:t>Fortschritt</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -177,7 +207,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.1948601860681439E-2"/>
+          <c:y val="9.2298103104225024E-2"/>
+          <c:w val="0.89809675246354881"/>
+          <c:h val="0.55442739643569816"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -208,11 +248,69 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$1:$A$5</c:f>
+              <c:f>Tabelle1!$A$1:$A$7</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Anfangsprogramm</c:v>
                 </c:pt>
@@ -220,23 +318,29 @@
                   <c:v>Anfangsprogramm mit Kopileroptimierung</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>initSpielfeld gelöscht</c:v>
+                  <c:v>initSpielefeld gelöscht</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>pruefeRegeln überarbeitet</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>X,Y Anzeige &amp; Lebende Anzeige entfert</c:v>
+                  <c:v>X,Y Anzeige links oben entfernt</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Zähllebende und FindNachbar zusammengefasst, Funktionsaufrufe entfernen</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Datentypen optimert, Funktionsaufruf pruefeRegeln entfernt</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$1:$B$5</c:f>
+              <c:f>Tabelle1!$B$1:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>56.3</c:v>
                 </c:pt>
@@ -252,6 +356,12 @@
                 <c:pt idx="4">
                   <c:v>24</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -263,8 +373,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -282,6 +393,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>Namen</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-AT" baseline="0"/>
+                  <a:t> der Commits</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-AT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -347,6 +518,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>benötigte Zeit für eine Generation</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-AT" baseline="0"/>
+                  <a:t> in sek</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-AT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -982,15 +1213,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>11430</xdr:rowOff>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>135254</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1016,10 +1247,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1288,64 +1515,81 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="71.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="2">
         <v>56.3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>40.4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>38.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>7.2</v>
+      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>5.3</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A7" r:id="rId1" tooltip="Datentypen optimert, Funktionsaufruf pruefeRegeln entfernt" display="https://github.com/minigimli/ConwaysGameSimulation/commit/3d118a9d46fc356c51df096d000bad11f0d5cf76" xr:uid="{F754EC2E-90ED-4D32-AEA3-9E65B02D0801}"/>
+    <hyperlink ref="A6" r:id="rId2" display="https://github.com/minigimli/ConwaysGameSimulation/commit/2551ff231fffd7e81e48790183b8706d08513050" xr:uid="{1FA7E6FA-1C7C-450D-B178-DAC10646461F}"/>
+    <hyperlink ref="A5" r:id="rId3" display="https://github.com/minigimli/ConwaysGameSimulation/commit/5d05ee1568541f61c88a64b95ffbddae64ee31fe" xr:uid="{E4BEEC4E-9015-4E29-AA94-72A1C59E7A1B}"/>
+    <hyperlink ref="A4" r:id="rId4" display="https://github.com/minigimli/ConwaysGameSimulation/commit/6dc1db2b1e0af43ffb269fe6d55971965dd51a72" xr:uid="{2588C90F-D2DC-41BB-B4EC-ADF2BCE8767A}"/>
+    <hyperlink ref="A3" r:id="rId5" display="https://github.com/minigimli/ConwaysGameSimulation/commit/3def1637ec3e7c020095b1e7598c177ee3b1c3ec" xr:uid="{C87A3D49-6868-445E-AA83-E2F0D29848A5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>